<commit_message>
Debugged Contrast Threshold Code
Seems ready to go.  Final testing on lab setup day.
</commit_message>
<xml_diff>
--- a/iMac Specs.xlsx
+++ b/iMac Specs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maunsell/Desktop/NSCI-20100 Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF00F193-D3D1-B442-A53F-FB8496334AB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D8A48AF-AB21-2D47-B4B0-C5B242C5FD62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="960" windowWidth="21200" windowHeight="17040" xr2:uid="{452F3D50-E6E0-7C46-8FC6-174ABBB47882}"/>
+    <workbookView xWindow="5360" yWindow="460" windowWidth="21200" windowHeight="17040" xr2:uid="{452F3D50-E6E0-7C46-8FC6-174ABBB47882}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="29">
   <si>
     <t>iMac Num.</t>
   </si>
@@ -106,6 +106,18 @@
   </si>
   <si>
     <t>Necessary Matlab Toolboxes</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>205.208.43.103</t>
+  </si>
+  <si>
+    <t>205.208.92.231</t>
+  </si>
+  <si>
+    <t>205.208.43.70</t>
   </si>
 </sst>
 </file>
@@ -477,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41D39542-3C5E-B74F-A138-63075B5879BB}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -488,10 +500,12 @@
     <col min="1" max="1" width="34" style="1" customWidth="1"/>
     <col min="2" max="5" width="10.83203125" style="1"/>
     <col min="6" max="6" width="16.33203125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="7" max="10" width="10.83203125" style="1"/>
+    <col min="11" max="11" width="15.5" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -522,8 +536,11 @@
       <c r="J1" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -555,7 +572,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -584,7 +601,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -613,7 +630,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -642,7 +659,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -670,8 +687,11 @@
       <c r="J6" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -699,8 +719,11 @@
       <c r="J7" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -719,8 +742,11 @@
       <c r="F8" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -749,7 +775,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -769,7 +795,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -798,7 +824,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -827,7 +853,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -856,7 +882,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -885,7 +911,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>

</xml_diff>